<commit_message>
cell values representing time and date will no longer be returned as strings, but as instances of their corresponding java types
</commit_message>
<xml_diff>
--- a/test/com/inet/excel/parser/files/various_data_types.xlsx
+++ b/test/com/inet/excel/parser/files/various_data_types.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mareks\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\ExcelJConnect\test\com\inet\excel\parser\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A95D02D-E691-4E75-A905-F2095032EF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EACF346-8534-45E2-B4D1-DD9876877FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="1935" windowWidth="21600" windowHeight="11385" xr2:uid="{C5C1358D-8E1D-40E9-8DF0-8F8CB4A4352E}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{C5C1358D-8E1D-40E9-8DF0-8F8CB4A4352E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,18 +24,12 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="169" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="170" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -74,16 +68,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -402,80 +392,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BFB459B-ED51-4288-AE11-F007C57386E5}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A6" sqref="A6:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>333</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
         <v>444</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
         <v>555</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>45220</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
-        <v>47837</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>0.51388888888888895</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
         <v>2.4</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="e">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="e">
         <f>1/0</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
         <f>A2+A3</f>
         <v>555</v>
       </c>

</xml_diff>